<commit_message>
added project latest files
</commit_message>
<xml_diff>
--- a/data/Dist_Finland_TC02.xlsx
+++ b/data/Dist_Finland_TC02.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>FinlandHomeURL</t>
   </si>
@@ -65,9 +65,6 @@
     <t>http://www.esri.fi</t>
   </si>
   <si>
-    <t xml:space="preserve">ArcGIS Platform </t>
-  </si>
-  <si>
     <t xml:space="preserve">ArcGISPlatform </t>
   </si>
   <si>
@@ -111,6 +108,12 @@
   </si>
   <si>
     <t>Tuki</t>
+  </si>
+  <si>
+    <t>ArcGIS Platform</t>
+  </si>
+  <si>
+    <t>Liity meihin</t>
   </si>
 </sst>
 </file>
@@ -467,8 +470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,7 +499,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1" t="s">
         <v>7</v>
@@ -517,28 +520,28 @@
         <v>11</v>
       </c>
       <c r="I1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="P1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -546,7 +549,7 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -561,34 +564,34 @@
         <v>4</v>
       </c>
       <c r="G2" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="H2" t="s">
         <v>6</v>
       </c>
       <c r="I2" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="J2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="P2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>